<commit_message>
Updating the EDA summary for each tank , in cluding the visualisations into the report
</commit_message>
<xml_diff>
--- a/Original Excel file EDA/Data Breakdown per tank.xlsx
+++ b/Original Excel file EDA/Data Breakdown per tank.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Thesis 2023\Capstone---CCT\Original Excel file EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1BA9BE-900B-4912-A556-B63D15FE5911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A315B2-3A39-43C7-A784-4BB1F1E1BAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{75E7B4C2-31F3-4177-BC38-2910F3C78903}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{75E7B4C2-31F3-4177-BC38-2910F3C78903}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank breakdown of data" sheetId="1" r:id="rId1"/>
     <sheet name="Ingredient details " sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="22MT descriptive statistics" sheetId="5" r:id="rId5"/>
+    <sheet name="23MT descriptive statistics" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="111">
   <si>
     <t xml:space="preserve">Production Tank </t>
   </si>
@@ -351,13 +353,37 @@
   </si>
   <si>
     <t>Tank</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23MT Tank Descriptive Statistics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22MT Tank Descriptive Statistics </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,8 +431,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,8 +464,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -501,11 +546,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -535,17 +626,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -554,6 +636,48 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1216,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EDC9EC-C51A-469D-A796-E3497185B44B}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
@@ -1228,10 +1352,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>89</v>
       </c>
       <c r="C1" s="18" t="s">
@@ -1243,23 +1367,23 @@
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1313,7 +1437,7 @@
       <c r="A5" s="2">
         <v>1002818</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>98</v>
       </c>
       <c r="C5" s="2">
@@ -1564,10 +1688,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1621,7 +1745,7 @@
       <c r="A4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="19" t="s">
         <v>83</v>
       </c>
       <c r="C4" s="10"/>
@@ -1644,7 +1768,7 @@
       <c r="A5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1665,7 +1789,7 @@
       <c r="A6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1686,7 +1810,7 @@
       <c r="A7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1707,7 +1831,7 @@
       <c r="A8" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1728,7 +1852,7 @@
       <c r="A9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1749,7 +1873,7 @@
       <c r="A10" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="20" t="s">
         <v>78</v>
       </c>
       <c r="C10" s="10"/>
@@ -1772,7 +1896,7 @@
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -1793,7 +1917,7 @@
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1906,7 +2030,7 @@
       <c r="A17" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>87</v>
       </c>
       <c r="C17" s="10"/>
@@ -1978,4 +2102,545 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401A5533-B6F3-4671-9DA8-75C276B4ED7A}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="23">
+        <v>73</v>
+      </c>
+      <c r="C3" s="23">
+        <v>73</v>
+      </c>
+      <c r="D3" s="23">
+        <v>73</v>
+      </c>
+      <c r="E3" s="23">
+        <v>73</v>
+      </c>
+      <c r="F3" s="23">
+        <v>73</v>
+      </c>
+      <c r="G3" s="23">
+        <v>67</v>
+      </c>
+      <c r="H3" s="23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="23">
+        <v>594.97260300000005</v>
+      </c>
+      <c r="C4" s="23">
+        <v>371.684932</v>
+      </c>
+      <c r="D4" s="23">
+        <v>2026.8493149999999</v>
+      </c>
+      <c r="E4" s="23">
+        <v>63.646039999999999</v>
+      </c>
+      <c r="F4" s="23">
+        <v>23.235994000000002</v>
+      </c>
+      <c r="G4" s="23">
+        <v>228.93580700000001</v>
+      </c>
+      <c r="H4" s="23">
+        <v>28611.7192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="23">
+        <v>615.81326000000001</v>
+      </c>
+      <c r="C5" s="23">
+        <v>584.61259399999994</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1954.7133260000001</v>
+      </c>
+      <c r="E5" s="23">
+        <v>35.450276000000002</v>
+      </c>
+      <c r="F5" s="23">
+        <v>15.59567</v>
+      </c>
+      <c r="G5" s="23">
+        <v>69.405963999999997</v>
+      </c>
+      <c r="H5" s="23">
+        <v>9629.4708009999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="23">
+        <v>93</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
+        <v>11.1</v>
+      </c>
+      <c r="G6" s="23">
+        <v>131.96080000000001</v>
+      </c>
+      <c r="H6" s="23">
+        <v>11151.564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="B7" s="23">
+        <v>205</v>
+      </c>
+      <c r="C7" s="23">
+        <v>25</v>
+      </c>
+      <c r="D7" s="23">
+        <v>9</v>
+      </c>
+      <c r="E7" s="23">
+        <v>36.774540000000002</v>
+      </c>
+      <c r="F7" s="23">
+        <v>15.588234999999999</v>
+      </c>
+      <c r="G7" s="23">
+        <v>188.249709</v>
+      </c>
+      <c r="H7" s="23">
+        <v>19857.794750000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="23">
+        <v>428</v>
+      </c>
+      <c r="C8" s="23">
+        <v>172</v>
+      </c>
+      <c r="D8" s="23">
+        <v>2186</v>
+      </c>
+      <c r="E8" s="23">
+        <v>68.392188000000004</v>
+      </c>
+      <c r="F8" s="23">
+        <v>17.411764999999999</v>
+      </c>
+      <c r="G8" s="23">
+        <v>237.85040000000001</v>
+      </c>
+      <c r="H8" s="23">
+        <v>32062.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="B9" s="23">
+        <v>750</v>
+      </c>
+      <c r="C9" s="23">
+        <v>380</v>
+      </c>
+      <c r="D9" s="23">
+        <v>3602</v>
+      </c>
+      <c r="E9" s="23">
+        <v>92.402843000000004</v>
+      </c>
+      <c r="F9" s="23">
+        <v>25.111111000000001</v>
+      </c>
+      <c r="G9" s="23">
+        <v>247.907363</v>
+      </c>
+      <c r="H9" s="23">
+        <v>37713.667000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="23">
+        <v>3356</v>
+      </c>
+      <c r="C10" s="23">
+        <v>3057</v>
+      </c>
+      <c r="D10" s="23">
+        <v>5474</v>
+      </c>
+      <c r="E10" s="23">
+        <v>127.688275</v>
+      </c>
+      <c r="F10" s="23">
+        <v>121.5</v>
+      </c>
+      <c r="G10" s="23">
+        <v>547.5</v>
+      </c>
+      <c r="H10" s="23">
+        <v>39978.798000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F224CA-9E61-4463-AECE-12EAB435F547}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="30">
+        <v>162</v>
+      </c>
+      <c r="C3" s="30">
+        <v>162</v>
+      </c>
+      <c r="D3" s="30">
+        <v>162</v>
+      </c>
+      <c r="E3" s="30">
+        <v>162</v>
+      </c>
+      <c r="F3" s="30">
+        <v>162</v>
+      </c>
+      <c r="G3" s="30">
+        <v>123</v>
+      </c>
+      <c r="H3" s="30">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="30">
+        <v>428.68518499999999</v>
+      </c>
+      <c r="C4" s="30">
+        <v>200.41358</v>
+      </c>
+      <c r="D4" s="30">
+        <v>1603.2654319999999</v>
+      </c>
+      <c r="E4" s="30">
+        <v>54.210925000000003</v>
+      </c>
+      <c r="F4" s="30">
+        <v>24.726596000000001</v>
+      </c>
+      <c r="G4" s="30">
+        <v>224.71793500000001</v>
+      </c>
+      <c r="H4" s="30">
+        <v>27760.113675000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="30">
+        <v>391.562049</v>
+      </c>
+      <c r="C5" s="30">
+        <v>292.99427900000001</v>
+      </c>
+      <c r="D5" s="30">
+        <v>1825.2382459999999</v>
+      </c>
+      <c r="E5" s="30">
+        <v>36.369574999999998</v>
+      </c>
+      <c r="F5" s="30">
+        <v>35.910556999999997</v>
+      </c>
+      <c r="G5" s="30">
+        <v>43.103060999999997</v>
+      </c>
+      <c r="H5" s="30">
+        <v>10206.042090999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="30">
+        <v>81</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
+        <v>2</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
+        <v>10.25</v>
+      </c>
+      <c r="G6" s="30">
+        <v>34.382649999999998</v>
+      </c>
+      <c r="H6" s="30">
+        <v>10217.813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="B7" s="30">
+        <v>161</v>
+      </c>
+      <c r="C7" s="30">
+        <v>4</v>
+      </c>
+      <c r="D7" s="30">
+        <v>6</v>
+      </c>
+      <c r="E7" s="30">
+        <v>33.774746</v>
+      </c>
+      <c r="F7" s="30">
+        <v>15.45</v>
+      </c>
+      <c r="G7" s="30">
+        <v>189.022435</v>
+      </c>
+      <c r="H7" s="30">
+        <v>18990.225999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="30">
+        <v>358</v>
+      </c>
+      <c r="C8" s="30">
+        <v>113.5</v>
+      </c>
+      <c r="D8" s="30">
+        <v>393.5</v>
+      </c>
+      <c r="E8" s="30">
+        <v>48.878549999999997</v>
+      </c>
+      <c r="F8" s="30">
+        <v>17.724637999999999</v>
+      </c>
+      <c r="G8" s="30">
+        <v>237.85040000000001</v>
+      </c>
+      <c r="H8" s="30">
+        <v>19945.525000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="B9" s="30">
+        <v>574</v>
+      </c>
+      <c r="C9" s="30">
+        <v>278.25</v>
+      </c>
+      <c r="D9" s="30">
+        <v>3303.25</v>
+      </c>
+      <c r="E9" s="30">
+        <v>86.704772000000006</v>
+      </c>
+      <c r="F9" s="30">
+        <v>31.866667</v>
+      </c>
+      <c r="G9" s="30">
+        <v>247.907363</v>
+      </c>
+      <c r="H9" s="30">
+        <v>38068.563999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="30">
+        <v>2749</v>
+      </c>
+      <c r="C10" s="30">
+        <v>2093</v>
+      </c>
+      <c r="D10" s="30">
+        <v>5535</v>
+      </c>
+      <c r="E10" s="30">
+        <v>112.882116</v>
+      </c>
+      <c r="F10" s="30">
+        <v>460.5</v>
+      </c>
+      <c r="G10" s="30">
+        <v>308.1123</v>
+      </c>
+      <c r="H10" s="30">
+        <v>56817.527999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating each of the tank notebooks with organised EDA
</commit_message>
<xml_diff>
--- a/Original Excel file EDA/Data Breakdown per tank.xlsx
+++ b/Original Excel file EDA/Data Breakdown per tank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Thesis 2023\Capstone---CCT\Original Excel file EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A315B2-3A39-43C7-A784-4BB1F1E1BAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C09D2-C2B4-4215-A0BB-620FCFD3C176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{75E7B4C2-31F3-4177-BC38-2910F3C78903}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{75E7B4C2-31F3-4177-BC38-2910F3C78903}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank breakdown of data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="22MT descriptive statistics" sheetId="5" r:id="rId5"/>
     <sheet name="23MT descriptive statistics" sheetId="6" r:id="rId6"/>
+    <sheet name="25MT4 descriptive statistics " sheetId="7" r:id="rId7"/>
+    <sheet name="25MT4 10escriptive statistics " sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="113">
   <si>
     <t xml:space="preserve">Production Tank </t>
   </si>
@@ -374,6 +376,12 @@
   </si>
   <si>
     <t xml:space="preserve">22MT Tank Descriptive Statistics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25MT4  Tank Descriptive Statistics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25MT10  Tank Descriptive Statistics </t>
   </si>
 </sst>
 </file>
@@ -596,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -677,6 +685,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2108,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401A5533-B6F3-4671-9DA8-75C276B4ED7A}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,4 +2672,545 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6F189F-3DD3-4C0E-BC83-876A931C5E0B}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="32">
+        <v>100</v>
+      </c>
+      <c r="C3" s="32">
+        <v>100</v>
+      </c>
+      <c r="D3" s="32">
+        <v>100</v>
+      </c>
+      <c r="E3" s="32">
+        <v>100</v>
+      </c>
+      <c r="F3" s="32">
+        <v>100</v>
+      </c>
+      <c r="G3" s="32">
+        <v>100</v>
+      </c>
+      <c r="H3" s="32">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="33">
+        <v>402.24</v>
+      </c>
+      <c r="C4" s="33">
+        <v>192.24</v>
+      </c>
+      <c r="D4" s="33">
+        <v>355.97</v>
+      </c>
+      <c r="E4" s="33">
+        <v>8.3820160000000001</v>
+      </c>
+      <c r="F4" s="33">
+        <v>24.341723000000002</v>
+      </c>
+      <c r="G4" s="33">
+        <v>52.630040000000001</v>
+      </c>
+      <c r="H4" s="33">
+        <v>5785.0519599999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="33">
+        <v>269.59071599999999</v>
+      </c>
+      <c r="C5" s="33">
+        <v>230.93473299999999</v>
+      </c>
+      <c r="D5" s="33">
+        <v>626.72190999999998</v>
+      </c>
+      <c r="E5" s="33">
+        <v>2.6326800000000001</v>
+      </c>
+      <c r="F5" s="33">
+        <v>12.903077</v>
+      </c>
+      <c r="G5" s="33">
+        <v>14.120573</v>
+      </c>
+      <c r="H5" s="33">
+        <v>978.92264899999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="33">
+        <v>160</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0.84933000000000003</v>
+      </c>
+      <c r="F6" s="33">
+        <v>6.4</v>
+      </c>
+      <c r="G6" s="33">
+        <v>28.128399999999999</v>
+      </c>
+      <c r="H6" s="33">
+        <v>2607.538024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="B7" s="33">
+        <v>226.75</v>
+      </c>
+      <c r="C7" s="33">
+        <v>65.75</v>
+      </c>
+      <c r="D7" s="33">
+        <v>4</v>
+      </c>
+      <c r="E7" s="33">
+        <v>6.7925800000000001</v>
+      </c>
+      <c r="F7" s="33">
+        <v>14.001785999999999</v>
+      </c>
+      <c r="G7" s="33">
+        <v>42.756799999999998</v>
+      </c>
+      <c r="H7" s="33">
+        <v>5405.1319999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="33">
+        <v>315.5</v>
+      </c>
+      <c r="C8" s="33">
+        <v>102.5</v>
+      </c>
+      <c r="D8" s="33">
+        <v>168</v>
+      </c>
+      <c r="E8" s="33">
+        <v>8.7131319999999999</v>
+      </c>
+      <c r="F8" s="33">
+        <v>16.973683999999999</v>
+      </c>
+      <c r="G8" s="33">
+        <v>52.028700000000001</v>
+      </c>
+      <c r="H8" s="33">
+        <v>5613.7039999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="B9" s="33">
+        <v>512</v>
+      </c>
+      <c r="C9" s="33">
+        <v>259.5</v>
+      </c>
+      <c r="D9" s="33">
+        <v>501.25</v>
+      </c>
+      <c r="E9" s="33">
+        <v>10.046334999999999</v>
+      </c>
+      <c r="F9" s="33">
+        <v>33.1</v>
+      </c>
+      <c r="G9" s="33">
+        <v>59.023000000000003</v>
+      </c>
+      <c r="H9" s="33">
+        <v>6409.4019520000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="33">
+        <v>2180</v>
+      </c>
+      <c r="C10" s="33">
+        <v>1874</v>
+      </c>
+      <c r="D10" s="33">
+        <v>4220</v>
+      </c>
+      <c r="E10" s="33">
+        <v>16.314109999999999</v>
+      </c>
+      <c r="F10" s="33">
+        <v>81</v>
+      </c>
+      <c r="G10" s="33">
+        <v>110</v>
+      </c>
+      <c r="H10" s="33">
+        <v>7250.4900980000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501615E-193D-4208-8969-BE220BC5E95F}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="37"/>
+      <c r="B1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="38">
+        <v>196</v>
+      </c>
+      <c r="C3" s="38">
+        <v>196</v>
+      </c>
+      <c r="D3" s="38">
+        <v>196</v>
+      </c>
+      <c r="E3" s="38">
+        <v>196</v>
+      </c>
+      <c r="F3" s="38">
+        <v>196</v>
+      </c>
+      <c r="G3" s="38">
+        <v>195</v>
+      </c>
+      <c r="H3" s="38">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="33">
+        <v>590.97448999999995</v>
+      </c>
+      <c r="C4" s="33">
+        <v>216.77551</v>
+      </c>
+      <c r="D4" s="33">
+        <v>299.08163300000001</v>
+      </c>
+      <c r="E4" s="33">
+        <v>14.895690999999999</v>
+      </c>
+      <c r="F4" s="33">
+        <v>42.798948000000003</v>
+      </c>
+      <c r="G4" s="33">
+        <v>91.814149999999998</v>
+      </c>
+      <c r="H4" s="33">
+        <v>15949.466639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="33">
+        <v>282.87975899999998</v>
+      </c>
+      <c r="C5" s="33">
+        <v>222.12412900000001</v>
+      </c>
+      <c r="D5" s="33">
+        <v>504.70842900000002</v>
+      </c>
+      <c r="E5" s="33">
+        <v>20.918087</v>
+      </c>
+      <c r="F5" s="33">
+        <v>24.343692999999998</v>
+      </c>
+      <c r="G5" s="33">
+        <v>36.735585999999998</v>
+      </c>
+      <c r="H5" s="33">
+        <v>3583.2547199999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="33">
+        <v>21</v>
+      </c>
+      <c r="C6" s="33">
+        <v>7</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1.3333330000000001</v>
+      </c>
+      <c r="G6" s="33">
+        <v>37.722749999999998</v>
+      </c>
+      <c r="H6" s="33">
+        <v>1764.0640000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="B7" s="33">
+        <v>383.75</v>
+      </c>
+      <c r="C7" s="33">
+        <v>60</v>
+      </c>
+      <c r="D7" s="33">
+        <v>4</v>
+      </c>
+      <c r="E7" s="33">
+        <v>10.988894999999999</v>
+      </c>
+      <c r="F7" s="33">
+        <v>21.990385</v>
+      </c>
+      <c r="G7" s="33">
+        <v>61.945500000000003</v>
+      </c>
+      <c r="H7" s="33">
+        <v>15805.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="33">
+        <v>500.5</v>
+      </c>
+      <c r="C8" s="33">
+        <v>124.5</v>
+      </c>
+      <c r="D8" s="33">
+        <v>63.5</v>
+      </c>
+      <c r="E8" s="33">
+        <v>11.728714</v>
+      </c>
+      <c r="F8" s="33">
+        <v>25.812864999999999</v>
+      </c>
+      <c r="G8" s="33">
+        <v>65.187236999999996</v>
+      </c>
+      <c r="H8" s="33">
+        <v>17565.838</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="B9" s="33">
+        <v>753.25</v>
+      </c>
+      <c r="C9" s="33">
+        <v>307</v>
+      </c>
+      <c r="D9" s="33">
+        <v>431.75</v>
+      </c>
+      <c r="E9" s="33">
+        <v>15.912818</v>
+      </c>
+      <c r="F9" s="33">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="G9" s="33">
+        <v>114.604816</v>
+      </c>
+      <c r="H9" s="33">
+        <v>18004.052</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="33">
+        <v>1865</v>
+      </c>
+      <c r="C10" s="33">
+        <v>1452</v>
+      </c>
+      <c r="D10" s="33">
+        <v>3051</v>
+      </c>
+      <c r="E10" s="33">
+        <v>296.83446800000002</v>
+      </c>
+      <c r="F10" s="33">
+        <v>151</v>
+      </c>
+      <c r="G10" s="33">
+        <v>195.86675</v>
+      </c>
+      <c r="H10" s="33">
+        <v>19979.646000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating working notebooks - 22MT creating better results and excel files for easy access to results for writeup
</commit_message>
<xml_diff>
--- a/Original Excel file EDA/Data Breakdown per tank.xlsx
+++ b/Original Excel file EDA/Data Breakdown per tank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Thesis 2023\Capstone---CCT\Original Excel file EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C09D2-C2B4-4215-A0BB-620FCFD3C176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134E9E36-8138-47FD-B47E-ACA5C59CCCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{75E7B4C2-31F3-4177-BC38-2910F3C78903}"/>
   </bookViews>
@@ -389,7 +389,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -645,6 +645,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -653,21 +686,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -681,18 +699,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -701,12 +707,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1387,13 +1387,13 @@
       <c r="B1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -1774,7 +1774,7 @@
       <c r="A4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="30" t="s">
         <v>83</v>
       </c>
       <c r="C4" s="10"/>
@@ -1797,7 +1797,7 @@
       <c r="A5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1818,7 +1818,7 @@
       <c r="A6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1839,7 +1839,7 @@
       <c r="A7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1860,7 +1860,7 @@
       <c r="A8" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1881,7 +1881,7 @@
       <c r="A9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1902,7 +1902,7 @@
       <c r="A10" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="31" t="s">
         <v>78</v>
       </c>
       <c r="C10" s="10"/>
@@ -1925,7 +1925,7 @@
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -1946,7 +1946,7 @@
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="20"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -2153,246 +2153,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="20">
         <v>73</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="20">
         <v>73</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="20">
         <v>73</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="20">
         <v>73</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>73</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>67</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="20">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="20">
         <v>594.97260300000005</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="20">
         <v>371.684932</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <v>2026.8493149999999</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="20">
         <v>63.646039999999999</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>23.235994000000002</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>228.93580700000001</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="20">
         <v>28611.7192</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="20">
         <v>615.81326000000001</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="20">
         <v>584.61259399999994</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>1954.7133260000001</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>35.450276000000002</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>15.59567</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>69.405963999999997</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="20">
         <v>9629.4708009999995</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="20">
         <v>93</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="20">
         <v>0</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>2</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>0</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>11.1</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>131.96080000000001</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="20">
         <v>11151.564</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="19">
         <v>0.25</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="20">
         <v>205</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="20">
         <v>25</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>9</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>36.774540000000002</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>15.588234999999999</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>188.249709</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="20">
         <v>19857.794750000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="19">
         <v>0.5</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="20">
         <v>428</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="20">
         <v>172</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>2186</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>68.392188000000004</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>17.411764999999999</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>237.85040000000001</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="20">
         <v>32062.17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="19">
         <v>0.75</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="20">
         <v>750</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="20">
         <v>380</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>3602</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <v>92.402843000000004</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>25.111111000000001</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>247.907363</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="20">
         <v>37713.667000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="20">
         <v>3356</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="20">
         <v>3057</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>5474</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>127.688275</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>121.5</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>547.5</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="20">
         <v>39978.798000000003</v>
       </c>
     </row>
@@ -2424,245 +2424,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="23">
         <v>162</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="23">
         <v>162</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="23">
         <v>162</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="23">
         <v>162</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="23">
         <v>162</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="23">
         <v>123</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="23">
         <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="23">
         <v>428.68518499999999</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="23">
         <v>200.41358</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="23">
         <v>1603.2654319999999</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="23">
         <v>54.210925000000003</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="23">
         <v>24.726596000000001</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="23">
         <v>224.71793500000001</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="23">
         <v>27760.113675000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="23">
         <v>391.562049</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="23">
         <v>292.99427900000001</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="23">
         <v>1825.2382459999999</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="23">
         <v>36.369574999999998</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="23">
         <v>35.910556999999997</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="23">
         <v>43.103060999999997</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="23">
         <v>10206.042090999999</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="23">
         <v>81</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="23">
         <v>0</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="23">
         <v>2</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="23">
         <v>0</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="23">
         <v>10.25</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="23">
         <v>34.382649999999998</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="23">
         <v>10217.813</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
+      <c r="A7" s="24">
         <v>0.25</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="23">
         <v>161</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="23">
         <v>4</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="23">
         <v>6</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="23">
         <v>33.774746</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="23">
         <v>15.45</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="23">
         <v>189.022435</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="23">
         <v>18990.225999999999</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
+      <c r="A8" s="24">
         <v>0.5</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="23">
         <v>358</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="23">
         <v>113.5</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="23">
         <v>393.5</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="23">
         <v>48.878549999999997</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="23">
         <v>17.724637999999999</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="23">
         <v>237.85040000000001</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="23">
         <v>19945.525000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="24">
         <v>0.75</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="23">
         <v>574</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="23">
         <v>278.25</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="23">
         <v>3303.25</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="23">
         <v>86.704772000000006</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="23">
         <v>31.866667</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="23">
         <v>247.907363</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="23">
         <v>38068.563999999998</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="23">
         <v>2749</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="23">
         <v>2093</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="23">
         <v>5535</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="23">
         <v>112.882116</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="23">
         <v>460.5</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="23">
         <v>308.1123</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="23">
         <v>56817.527999999998</v>
       </c>
     </row>
@@ -2693,246 +2693,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="25">
         <v>100</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="25">
         <v>100</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="25">
         <v>100</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="25">
         <v>100</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="25">
         <v>100</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="25">
         <v>100</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="25">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="26">
         <v>402.24</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="26">
         <v>192.24</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="26">
         <v>355.97</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="26">
         <v>8.3820160000000001</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="26">
         <v>24.341723000000002</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="26">
         <v>52.630040000000001</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="26">
         <v>5785.0519599999998</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="26">
         <v>269.59071599999999</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="26">
         <v>230.93473299999999</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="26">
         <v>626.72190999999998</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="26">
         <v>2.6326800000000001</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="26">
         <v>12.903077</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="26">
         <v>14.120573</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="26">
         <v>978.92264899999998</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="26">
         <v>160</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="26">
         <v>0</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="26">
         <v>1</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="26">
         <v>0.84933000000000003</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="26">
         <v>6.4</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="26">
         <v>28.128399999999999</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="26">
         <v>2607.538024</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
+      <c r="A7" s="24">
         <v>0.25</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="26">
         <v>226.75</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="26">
         <v>65.75</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="26">
         <v>4</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="26">
         <v>6.7925800000000001</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="26">
         <v>14.001785999999999</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="26">
         <v>42.756799999999998</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="26">
         <v>5405.1319999999996</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
+      <c r="A8" s="24">
         <v>0.5</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="26">
         <v>315.5</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="26">
         <v>102.5</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="26">
         <v>168</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="26">
         <v>8.7131319999999999</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="26">
         <v>16.973683999999999</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="26">
         <v>52.028700000000001</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="26">
         <v>5613.7039999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="24">
         <v>0.75</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="26">
         <v>512</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="26">
         <v>259.5</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="26">
         <v>501.25</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="26">
         <v>10.046334999999999</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="26">
         <v>33.1</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="26">
         <v>59.023000000000003</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="26">
         <v>6409.4019520000002</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="26">
         <v>2180</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="26">
         <v>1874</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="26">
         <v>4220</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="26">
         <v>16.314109999999999</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="26">
         <v>81</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="26">
         <v>110</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="26">
         <v>7250.4900980000002</v>
       </c>
     </row>
@@ -2964,246 +2964,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="28">
         <v>196</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="28">
         <v>196</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="28">
         <v>196</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="28">
         <v>196</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="28">
         <v>196</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="28">
         <v>195</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="28">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="26">
         <v>590.97448999999995</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="26">
         <v>216.77551</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="26">
         <v>299.08163300000001</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="26">
         <v>14.895690999999999</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="26">
         <v>42.798948000000003</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="26">
         <v>91.814149999999998</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="26">
         <v>15949.466639</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="26">
         <v>282.87975899999998</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="26">
         <v>222.12412900000001</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="26">
         <v>504.70842900000002</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="26">
         <v>20.918087</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="26">
         <v>24.343692999999998</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="26">
         <v>36.735585999999998</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="26">
         <v>3583.2547199999999</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="26">
         <v>21</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="26">
         <v>7</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="26">
         <v>0</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="26">
         <v>0</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="26">
         <v>1.3333330000000001</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="26">
         <v>37.722749999999998</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="26">
         <v>1764.0640000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
+      <c r="A7" s="24">
         <v>0.25</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="26">
         <v>383.75</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="26">
         <v>60</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="26">
         <v>4</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="26">
         <v>10.988894999999999</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="26">
         <v>21.990385</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="26">
         <v>61.945500000000003</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="26">
         <v>15805.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
+      <c r="A8" s="24">
         <v>0.5</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="26">
         <v>500.5</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="26">
         <v>124.5</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="26">
         <v>63.5</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="26">
         <v>11.728714</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="26">
         <v>25.812864999999999</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="26">
         <v>65.187236999999996</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="26">
         <v>17565.838</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="24">
         <v>0.75</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="26">
         <v>753.25</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="26">
         <v>307</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="26">
         <v>431.75</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="26">
         <v>15.912818</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="26">
         <v>66.599999999999994</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="26">
         <v>114.604816</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="26">
         <v>18004.052</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="26">
         <v>1865</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="26">
         <v>1452</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="26">
         <v>3051</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="26">
         <v>296.83446800000002</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="26">
         <v>151</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="26">
         <v>195.86675</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="26">
         <v>19979.646000000001</v>
       </c>
     </row>

</xml_diff>